<commit_message>
Changed the demands, efficiencies and capacities
</commit_message>
<xml_diff>
--- a/VT_SHR_RCI_V01.xlsx
+++ b/VT_SHR_RCI_V01.xlsx
@@ -1556,7 +1556,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1602,6 +1602,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="11"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1673,7 +1679,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1807,6 +1813,8 @@
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3730,8 +3738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AD69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4022,8 +4030,9 @@
       </c>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
-      <c r="J11" s="17">
-        <v>2.25</v>
+      <c r="J11" s="68">
+        <f>1000/(120*3.6)</f>
+        <v>2.3148148148148149</v>
       </c>
       <c r="K11" s="17">
         <v>100</v>
@@ -4076,8 +4085,9 @@
       </c>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
-      <c r="J12" s="17">
-        <v>30</v>
+      <c r="J12" s="68">
+        <f>J11*3</f>
+        <v>6.9444444444444446</v>
       </c>
       <c r="K12" s="17">
         <v>100</v>
@@ -4130,8 +4140,9 @@
       </c>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
-      <c r="J13" s="17">
-        <v>9.6</v>
+      <c r="J13" s="68">
+        <f>J12</f>
+        <v>6.9444444444444446</v>
       </c>
       <c r="K13" s="17">
         <v>100</v>
@@ -4184,8 +4195,9 @@
       </c>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
-      <c r="J14" s="17">
-        <v>2</v>
+      <c r="J14" s="68">
+        <f>J11*1.01</f>
+        <v>2.3379629629629632</v>
       </c>
       <c r="K14" s="17">
         <v>100</v>
@@ -4238,8 +4250,9 @@
       </c>
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
-      <c r="J15" s="17">
-        <v>20</v>
+      <c r="J15" s="68">
+        <f t="shared" ref="J15:J16" si="0">J12*1.01</f>
+        <v>7.0138888888888893</v>
       </c>
       <c r="K15" s="17">
         <v>100</v>
@@ -4292,8 +4305,9 @@
       </c>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
-      <c r="J16" s="17">
-        <v>9.3000000000000007</v>
+      <c r="J16" s="68">
+        <f t="shared" si="0"/>
+        <v>7.0138888888888893</v>
       </c>
       <c r="K16" s="17">
         <v>100</v>
@@ -4455,7 +4469,7 @@
       <c r="H19" s="17"/>
       <c r="I19" s="32"/>
       <c r="J19" s="17">
-        <v>183</v>
+        <v>100</v>
       </c>
       <c r="K19" s="17">
         <v>100</v>
@@ -4566,7 +4580,7 @@
         <v>20</v>
       </c>
       <c r="L21" s="17">
-        <f t="shared" ref="L21:L30" si="0">8760*3.6/1000000</f>
+        <f t="shared" ref="L21:L30" si="1">8760*3.6/1000000</f>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="M21" s="17"/>
@@ -4619,7 +4633,7 @@
         <v>20</v>
       </c>
       <c r="L22" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="M22" s="17"/>
@@ -4672,7 +4686,7 @@
         <v>20</v>
       </c>
       <c r="L23" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="M23" s="17"/>
@@ -4725,7 +4739,7 @@
         <v>20</v>
       </c>
       <c r="L24" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="M24" s="17"/>
@@ -4765,7 +4779,7 @@
         <v>20</v>
       </c>
       <c r="L25" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="M25" s="17"/>
@@ -4805,7 +4819,7 @@
         <v>20</v>
       </c>
       <c r="L26" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="M26" s="17"/>
@@ -4845,7 +4859,7 @@
         <v>20</v>
       </c>
       <c r="L27" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="M27" s="17"/>
@@ -4886,7 +4900,7 @@
         <v>20</v>
       </c>
       <c r="L28" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="M28" s="38"/>
@@ -4894,7 +4908,7 @@
         <v>0.2</v>
       </c>
       <c r="O28" s="17">
-        <v>2200</v>
+        <v>1000</v>
       </c>
       <c r="P28" s="38"/>
     </row>
@@ -4927,7 +4941,7 @@
         <v>20</v>
       </c>
       <c r="L29" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="M29" s="38"/>
@@ -4968,7 +4982,7 @@
         <v>20</v>
       </c>
       <c r="L30" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="M30" s="38"/>
@@ -4976,7 +4990,7 @@
         <v>0.2</v>
       </c>
       <c r="O30" s="17">
-        <v>1700</v>
+        <v>1000</v>
       </c>
       <c r="P30" s="38"/>
     </row>
@@ -5353,8 +5367,8 @@
         <f>SEC_Comm!F10</f>
         <v>Mm2</v>
       </c>
-      <c r="E48" s="17">
-        <v>20</v>
+      <c r="E48" s="67">
+        <v>10</v>
       </c>
       <c r="F48" s="17"/>
       <c r="H48" s="65"/>
@@ -5378,7 +5392,8 @@
         <v>Mm2</v>
       </c>
       <c r="E49" s="17">
-        <v>20</v>
+        <f>E48</f>
+        <v>10</v>
       </c>
       <c r="F49" s="17"/>
       <c r="H49" s="65"/>
@@ -5402,7 +5417,8 @@
         <v>Mm2</v>
       </c>
       <c r="E50" s="17">
-        <v>20</v>
+        <f>E49</f>
+        <v>10</v>
       </c>
       <c r="F50" s="17"/>
       <c r="H50" s="65"/>
@@ -5425,8 +5441,8 @@
         <f>SEC_Comm!F13</f>
         <v>Mm2</v>
       </c>
-      <c r="E51" s="17">
-        <v>20</v>
+      <c r="E51" s="67">
+        <v>10</v>
       </c>
       <c r="F51" s="17"/>
       <c r="H51" s="65"/>
@@ -5498,7 +5514,7 @@
         <v>Mm2</v>
       </c>
       <c r="E54" s="17">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F54" s="17"/>
       <c r="H54" s="65"/>
@@ -5522,7 +5538,7 @@
         <v>Mm2</v>
       </c>
       <c r="E55" s="17">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F55" s="17"/>
       <c r="H55" s="65"/>

</xml_diff>

<commit_message>
Deleted demands from the SUP file and changed WCH to WPE
</commit_message>
<xml_diff>
--- a/VT_SHR_RCI_V01.xlsx
+++ b/VT_SHR_RCI_V01.xlsx
@@ -2324,8 +2324,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:S39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3738,8 +3738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AD69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4360,8 +4360,9 @@
       </c>
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
-      <c r="J17" s="17">
-        <v>1</v>
+      <c r="J17" s="68">
+        <f>J14</f>
+        <v>2.3379629629629632</v>
       </c>
       <c r="K17" s="17">
         <v>100</v>
@@ -4414,8 +4415,9 @@
       </c>
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
-      <c r="J18" s="17">
-        <v>2</v>
+      <c r="J18" s="68">
+        <f>J16</f>
+        <v>7.0138888888888893</v>
       </c>
       <c r="K18" s="17">
         <v>100</v>
@@ -5466,7 +5468,7 @@
         <v>Mm2</v>
       </c>
       <c r="E52" s="17">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F52" s="17"/>
       <c r="H52" s="65"/>
@@ -5490,7 +5492,7 @@
         <v>Mm2</v>
       </c>
       <c r="E53" s="17">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F53" s="17"/>
       <c r="H53" s="65"/>
@@ -5538,6 +5540,7 @@
         <v>Mm2</v>
       </c>
       <c r="E55" s="17">
+        <f>E54</f>
         <v>20</v>
       </c>
       <c r="F55" s="17"/>

</xml_diff>

<commit_message>
Changed the demands (in Mm2) and efficiencies
</commit_message>
<xml_diff>
--- a/VT_SHR_RCI_V01.xlsx
+++ b/VT_SHR_RCI_V01.xlsx
@@ -2324,8 +2324,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:S39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3738,8 +3738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AD69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4360,8 +4360,9 @@
       </c>
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
-      <c r="J17" s="17">
-        <v>1</v>
+      <c r="J17" s="68">
+        <f>J14</f>
+        <v>2.3379629629629632</v>
       </c>
       <c r="K17" s="17">
         <v>100</v>
@@ -4414,8 +4415,9 @@
       </c>
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
-      <c r="J18" s="17">
-        <v>2</v>
+      <c r="J18" s="68">
+        <f>J16</f>
+        <v>7.0138888888888893</v>
       </c>
       <c r="K18" s="17">
         <v>100</v>
@@ -5466,7 +5468,7 @@
         <v>Mm2</v>
       </c>
       <c r="E52" s="17">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F52" s="17"/>
       <c r="H52" s="65"/>
@@ -5490,7 +5492,7 @@
         <v>Mm2</v>
       </c>
       <c r="E53" s="17">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F53" s="17"/>
       <c r="H53" s="65"/>
@@ -5538,6 +5540,7 @@
         <v>Mm2</v>
       </c>
       <c r="E55" s="17">
+        <f>E54</f>
         <v>20</v>
       </c>
       <c r="F55" s="17"/>

</xml_diff>

<commit_message>
Changed RCI sector as suggested by Stefan
</commit_message>
<xml_diff>
--- a/VT_SHR_RCI_V01.xlsx
+++ b/VT_SHR_RCI_V01.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stpet\Git models\TIMES-SHIRE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jactat\Documents\Models\TIMES-Shire\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9555" yWindow="-15" windowWidth="9600" windowHeight="11640" tabRatio="901" activeTab="2"/>
+    <workbookView xWindow="9552" yWindow="-12" windowWidth="9600" windowHeight="11640" tabRatio="901" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SEC_Comm" sheetId="112" r:id="rId1"/>
@@ -23,7 +23,7 @@
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1496,7 +1496,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0;\-0.0;0"/>
     <numFmt numFmtId="165" formatCode="\Te\x\t"/>
@@ -2867,19 +2867,19 @@
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="50.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="50.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2888,13 +2888,13 @@
       </c>
       <c r="C1" s="24"/>
     </row>
-    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="17"/>
     </row>
-    <row r="6" spans="2:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B6" s="58" t="s">
         <v>43</v>
       </c>
@@ -2907,7 +2907,7 @@
       <c r="I6" s="60"/>
       <c r="J6" s="60"/>
     </row>
-    <row r="7" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="61" t="s">
         <v>14</v>
       </c>
@@ -2920,7 +2920,7 @@
       <c r="I7" s="60"/>
       <c r="J7" s="60"/>
     </row>
-    <row r="8" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="62" t="s">
         <v>7</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="65" t="s">
         <v>49</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="67" t="s">
         <v>94</v>
       </c>
@@ -2997,7 +2997,7 @@
       <c r="I10" s="67"/>
       <c r="J10" s="67"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="67"/>
       <c r="C11" s="67"/>
       <c r="D11" s="67" t="s">
@@ -3014,7 +3014,7 @@
       <c r="I11" s="67"/>
       <c r="J11" s="67"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="67"/>
       <c r="C12" s="67"/>
       <c r="D12" s="67" t="s">
@@ -3031,7 +3031,7 @@
       <c r="I12" s="67"/>
       <c r="J12" s="67"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="67"/>
       <c r="C13" s="67"/>
       <c r="D13" s="67" t="s">
@@ -3048,7 +3048,7 @@
       <c r="I13" s="67"/>
       <c r="J13" s="67"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="67"/>
       <c r="C14" s="67"/>
       <c r="D14" s="67" t="s">
@@ -3065,7 +3065,7 @@
       <c r="I14" s="67"/>
       <c r="J14" s="67"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="67"/>
       <c r="C15" s="67"/>
       <c r="D15" s="67" t="s">
@@ -3082,7 +3082,7 @@
       <c r="I15" s="67"/>
       <c r="J15" s="67"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="67"/>
       <c r="C16" s="67"/>
       <c r="D16" s="67" t="s">
@@ -3099,7 +3099,7 @@
       <c r="I16" s="67"/>
       <c r="J16" s="67"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="67"/>
       <c r="C17" s="67"/>
       <c r="D17" s="67" t="s">
@@ -3117,7 +3117,7 @@
       <c r="J17" s="67"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="68"/>
       <c r="C18" s="68"/>
       <c r="D18" s="69" t="s">
@@ -3134,7 +3134,7 @@
       <c r="I18" s="68"/>
       <c r="J18" s="68"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="67" t="s">
         <v>63</v>
       </c>
@@ -3153,7 +3153,7 @@
       <c r="I19" s="67"/>
       <c r="J19" s="67"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="67"/>
       <c r="C20" s="67"/>
       <c r="D20" s="70" t="s">
@@ -3170,7 +3170,7 @@
       <c r="I20" s="67"/>
       <c r="J20" s="67"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="67"/>
       <c r="C21" s="67"/>
       <c r="D21" s="70" t="s">
@@ -3191,7 +3191,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="67"/>
       <c r="C22" s="67"/>
       <c r="D22" s="70" t="s">
@@ -3212,7 +3212,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="67"/>
       <c r="C23" s="67"/>
       <c r="D23" s="70" t="s">
@@ -3231,7 +3231,7 @@
       <c r="I23" s="67"/>
       <c r="J23" s="67"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="67"/>
       <c r="C24" s="67"/>
       <c r="D24" s="70" t="s">
@@ -3250,7 +3250,7 @@
       <c r="I24" s="67"/>
       <c r="J24" s="67"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="67"/>
       <c r="C25" s="67"/>
       <c r="D25" s="70" t="s">
@@ -3269,7 +3269,7 @@
       <c r="I25" s="67"/>
       <c r="J25" s="67"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="67"/>
       <c r="C26" s="67"/>
       <c r="D26" s="70" t="s">
@@ -3288,7 +3288,7 @@
       <c r="I26" s="67"/>
       <c r="J26" s="67"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="67"/>
       <c r="C27" s="67"/>
       <c r="D27" s="67" t="s">
@@ -3307,7 +3307,7 @@
       <c r="I27" s="67"/>
       <c r="J27" s="67"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="67"/>
       <c r="C28" s="67"/>
       <c r="D28" s="67" t="s">
@@ -3326,7 +3326,7 @@
       <c r="I28" s="67"/>
       <c r="J28" s="67"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="67"/>
       <c r="C29" s="67"/>
       <c r="D29" s="67" t="s">
@@ -3345,7 +3345,7 @@
       <c r="I29" s="67"/>
       <c r="J29" s="67"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="67"/>
       <c r="C30" s="67"/>
       <c r="D30" s="70" t="s">
@@ -3366,7 +3366,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="67"/>
       <c r="C31" s="67"/>
       <c r="D31" s="70" t="s">
@@ -3385,7 +3385,7 @@
       <c r="I31" s="67"/>
       <c r="J31" s="67"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="67"/>
       <c r="C32" s="67"/>
       <c r="D32" s="70" t="s">
@@ -3404,7 +3404,7 @@
       <c r="I32" s="67"/>
       <c r="J32" s="67"/>
     </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B33" s="67"/>
       <c r="C33" s="67"/>
       <c r="D33" s="70" t="s">
@@ -3423,7 +3423,7 @@
       <c r="I33" s="67"/>
       <c r="J33" s="67"/>
     </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B34" s="67"/>
       <c r="C34" s="67"/>
       <c r="D34" s="70" t="s">
@@ -3450,7 +3450,7 @@
       <c r="R34" s="56"/>
       <c r="S34" s="56"/>
     </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B35" s="67"/>
       <c r="C35" s="67"/>
       <c r="D35" s="70" t="s">
@@ -3479,7 +3479,7 @@
       <c r="R35" s="56"/>
       <c r="S35" s="56"/>
     </row>
-    <row r="36" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B36" s="67"/>
       <c r="C36" s="67"/>
       <c r="D36" s="67" t="s">
@@ -3506,7 +3506,7 @@
       <c r="R36" s="56"/>
       <c r="S36" s="56"/>
     </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B37" s="71" t="s">
         <v>87</v>
       </c>
@@ -3525,7 +3525,7 @@
       <c r="I37" s="71"/>
       <c r="J37" s="71"/>
     </row>
-    <row r="38" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B38" s="67"/>
       <c r="C38" s="67"/>
       <c r="D38" s="70" t="s">
@@ -3542,7 +3542,7 @@
       <c r="I38" s="67"/>
       <c r="J38" s="67"/>
     </row>
-    <row r="39" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B39" s="67"/>
       <c r="C39" s="67"/>
       <c r="D39" s="70" t="s">
@@ -3576,32 +3576,32 @@
       <selection activeCell="E36" sqref="E35:E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="65.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="65.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B1" s="24" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="58" t="s">
         <v>44</v>
@@ -3615,7 +3615,7 @@
       <c r="I5" s="73"/>
       <c r="J5" s="73"/>
     </row>
-    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="61" t="s">
         <v>16</v>
       </c>
@@ -3628,7 +3628,7 @@
       <c r="I6" s="73"/>
       <c r="J6" s="73"/>
     </row>
-    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="63" t="s">
         <v>11</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="66" t="s">
         <v>50</v>
       </c>
@@ -3686,7 +3686,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="70" t="s">
         <v>95</v>
       </c>
@@ -3707,7 +3707,7 @@
       <c r="I9" s="70"/>
       <c r="J9" s="70"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="70"/>
       <c r="C10" s="70"/>
       <c r="D10" s="67" t="s">
@@ -3726,7 +3726,7 @@
       <c r="I10" s="70"/>
       <c r="J10" s="70"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="70"/>
       <c r="C11" s="70"/>
       <c r="D11" s="67" t="s">
@@ -3745,7 +3745,7 @@
       <c r="I11" s="70"/>
       <c r="J11" s="70"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="70"/>
       <c r="C12" s="70"/>
       <c r="D12" s="67" t="s">
@@ -3764,7 +3764,7 @@
       <c r="I12" s="70"/>
       <c r="J12" s="70"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="70"/>
       <c r="C13" s="70"/>
       <c r="D13" s="67" t="s">
@@ -3783,7 +3783,7 @@
       <c r="I13" s="70"/>
       <c r="J13" s="70"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="70"/>
       <c r="C14" s="70"/>
       <c r="D14" s="67" t="s">
@@ -3802,7 +3802,7 @@
       <c r="I14" s="70"/>
       <c r="J14" s="70"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="70"/>
       <c r="C15" s="70"/>
       <c r="D15" s="67" t="s">
@@ -3821,7 +3821,7 @@
       <c r="I15" s="70"/>
       <c r="J15" s="70"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="70"/>
       <c r="C16" s="70"/>
       <c r="D16" s="67" t="s">
@@ -3840,7 +3840,7 @@
       <c r="I16" s="70"/>
       <c r="J16" s="70"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="70"/>
       <c r="C17" s="70"/>
       <c r="D17" s="67" t="s">
@@ -3859,7 +3859,7 @@
       <c r="I17" s="70"/>
       <c r="J17" s="70"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="72" t="s">
         <v>98</v>
       </c>
@@ -3882,7 +3882,7 @@
       <c r="I18" s="72"/>
       <c r="J18" s="72"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="70"/>
       <c r="C19" s="70"/>
       <c r="D19" s="70" t="s">
@@ -3903,7 +3903,7 @@
       <c r="I19" s="70"/>
       <c r="J19" s="70"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="70"/>
       <c r="C20" s="70"/>
       <c r="D20" s="70" t="s">
@@ -3924,7 +3924,7 @@
       <c r="I20" s="70"/>
       <c r="J20" s="70"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="70"/>
       <c r="C21" s="70"/>
       <c r="D21" s="70" t="s">
@@ -3945,7 +3945,7 @@
       <c r="I21" s="70"/>
       <c r="J21" s="70"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="70"/>
       <c r="C22" s="70"/>
       <c r="D22" s="70" t="s">
@@ -3966,7 +3966,7 @@
       <c r="I22" s="70"/>
       <c r="J22" s="70"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="70"/>
       <c r="C23" s="70"/>
       <c r="D23" s="70" t="s">
@@ -3987,7 +3987,7 @@
       <c r="I23" s="70"/>
       <c r="J23" s="70"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="70"/>
       <c r="C24" s="70"/>
       <c r="D24" s="70" t="s">
@@ -4008,7 +4008,7 @@
       <c r="I24" s="70"/>
       <c r="J24" s="70"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="70"/>
       <c r="C25" s="70"/>
       <c r="D25" s="70" t="s">
@@ -4029,7 +4029,7 @@
       <c r="I25" s="70"/>
       <c r="J25" s="70"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="70"/>
       <c r="C26" s="70"/>
       <c r="D26" s="70" t="s">
@@ -4050,7 +4050,7 @@
       <c r="I26" s="70"/>
       <c r="J26" s="70"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="70"/>
       <c r="C27" s="70"/>
       <c r="D27" s="70" t="s">
@@ -4071,7 +4071,7 @@
       <c r="I27" s="70"/>
       <c r="J27" s="70"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="70"/>
       <c r="C28" s="70"/>
       <c r="D28" s="67" t="s">
@@ -4092,7 +4092,7 @@
       <c r="I28" s="70"/>
       <c r="J28" s="70"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="70"/>
       <c r="C29" s="70"/>
       <c r="D29" s="70" t="s">
@@ -4111,7 +4111,7 @@
       <c r="I29" s="70"/>
       <c r="J29" s="70"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="72"/>
       <c r="C30" s="72"/>
       <c r="D30" s="72" t="s">
@@ -4132,7 +4132,7 @@
       <c r="I30" s="72"/>
       <c r="J30" s="72"/>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="70"/>
       <c r="C31" s="70"/>
       <c r="D31" s="70" t="s">
@@ -4153,7 +4153,7 @@
       <c r="I31" s="70"/>
       <c r="J31" s="70"/>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="70"/>
       <c r="C32" s="70"/>
       <c r="D32" s="70" t="s">
@@ -4174,7 +4174,7 @@
       <c r="I32" s="70"/>
       <c r="J32" s="70"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="70"/>
       <c r="C33" s="70"/>
       <c r="D33" s="70" t="s">
@@ -4195,7 +4195,7 @@
       <c r="I33" s="70"/>
       <c r="J33" s="70"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="70"/>
       <c r="C34" s="70"/>
       <c r="D34" s="70" t="s">
@@ -4216,7 +4216,7 @@
       <c r="I34" s="70"/>
       <c r="J34" s="70"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="70"/>
       <c r="C35" s="70"/>
       <c r="D35" s="70" t="s">
@@ -4237,7 +4237,7 @@
       <c r="I35" s="70"/>
       <c r="J35" s="70"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="70"/>
       <c r="C36" s="70"/>
       <c r="D36" s="70" t="s">
@@ -4258,7 +4258,7 @@
       <c r="I36" s="70"/>
       <c r="J36" s="70"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="70"/>
       <c r="C37" s="70"/>
       <c r="D37" s="70" t="s">
@@ -4292,53 +4292,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AD69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+    <sheetView tabSelected="1" topLeftCell="M9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="69.85546875" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="9" width="13.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="69.88671875" customWidth="1"/>
+    <col min="4" max="4" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" customWidth="1"/>
+    <col min="8" max="9" width="13.88671875" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" customWidth="1"/>
-    <col min="19" max="19" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.42578125" customWidth="1"/>
-    <col min="22" max="22" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.5546875" customWidth="1"/>
+    <col min="19" max="19" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.44140625" customWidth="1"/>
+    <col min="22" max="22" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:30" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:30" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B1" s="24" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="2:30" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:30" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:30" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
         <v>54</v>
       </c>
@@ -4359,7 +4359,7 @@
       <c r="AC5" s="34"/>
       <c r="AD5" s="34"/>
     </row>
-    <row r="6" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="2"/>
       <c r="E6" s="4"/>
@@ -4386,7 +4386,7 @@
       <c r="AC6" s="34"/>
       <c r="AD6" s="34"/>
     </row>
-    <row r="7" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:30" x14ac:dyDescent="0.25">
       <c r="H7" s="21" t="s">
         <v>13</v>
       </c>
@@ -4413,7 +4413,7 @@
       <c r="AC7" s="23"/>
       <c r="AD7" s="20"/>
     </row>
-    <row r="8" spans="2:30" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:30" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="27" t="s">
         <v>1</v>
       </c>
@@ -4473,7 +4473,7 @@
       <c r="AC8" s="41"/>
       <c r="AD8" s="41"/>
     </row>
-    <row r="9" spans="2:30" ht="42.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:30" ht="42.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14" t="s">
         <v>51</v>
       </c>
@@ -4529,7 +4529,7 @@
       <c r="AC9" s="32"/>
       <c r="AD9" s="32"/>
     </row>
-    <row r="10" spans="2:30" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:30" ht="12.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="29" t="s">
         <v>135</v>
       </c>
@@ -4567,7 +4567,7 @@
       <c r="AC10" s="32"/>
       <c r="AD10" s="32"/>
     </row>
-    <row r="11" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="str">
         <f>SEC_Processes!D9</f>
         <v>RHDDB</v>
@@ -4630,7 +4630,7 @@
       <c r="AC11" s="81"/>
       <c r="AD11" s="33"/>
     </row>
-    <row r="12" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="str">
         <f>SEC_Processes!D10</f>
         <v>RCDDB</v>
@@ -4693,7 +4693,7 @@
       <c r="AC12" s="83"/>
       <c r="AD12" s="33"/>
     </row>
-    <row r="13" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="str">
         <f>SEC_Processes!D11</f>
         <v>REDDB</v>
@@ -4744,7 +4744,7 @@
         <v>19</v>
       </c>
       <c r="V13" s="33">
-        <f t="shared" si="1"/>
+        <f>E50</f>
         <v>19</v>
       </c>
       <c r="W13" s="33"/>
@@ -4756,7 +4756,7 @@
       <c r="AC13" s="83"/>
       <c r="AD13" s="33"/>
     </row>
-    <row r="14" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="str">
         <f>SEC_Processes!D12</f>
         <v>RHDMB</v>
@@ -4819,7 +4819,7 @@
       <c r="AC14" s="83"/>
       <c r="AD14" s="33"/>
     </row>
-    <row r="15" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="str">
         <f>SEC_Processes!D13</f>
         <v>RCDMB</v>
@@ -4882,7 +4882,7 @@
       <c r="AC15" s="83"/>
       <c r="AD15" s="33"/>
     </row>
-    <row r="16" spans="2:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:30" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="12" t="str">
         <f>SEC_Processes!D14</f>
         <v>REDMB</v>
@@ -4945,7 +4945,7 @@
       <c r="AC16" s="85"/>
       <c r="AD16" s="34"/>
     </row>
-    <row r="17" spans="2:30" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:30" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="str">
         <f>SEC_Processes!D15</f>
         <v>CHDRB</v>
@@ -5008,7 +5008,7 @@
       <c r="AC17" s="85"/>
       <c r="AD17" s="34"/>
     </row>
-    <row r="18" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="str">
         <f>SEC_Processes!D16</f>
         <v>CCDRB</v>
@@ -5071,7 +5071,7 @@
       <c r="AC18" s="85"/>
       <c r="AD18" s="34"/>
     </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="str">
         <f>SEC_Processes!D17</f>
         <v>IPPDT</v>
@@ -5125,7 +5125,7 @@
       <c r="AC19" s="85"/>
       <c r="AD19" s="34"/>
     </row>
-    <row r="20" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B20" s="44" t="str">
         <f>SEC_Processes!D18</f>
         <v>RHTDBWPEBE1</v>
@@ -5178,7 +5178,7 @@
       <c r="AC20" s="85"/>
       <c r="AD20" s="34"/>
     </row>
-    <row r="21" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="str">
         <f>SEC_Processes!D19</f>
         <v>RHTMBWPEBE1</v>
@@ -5234,7 +5234,7 @@
       <c r="AC21" s="85"/>
       <c r="AD21" s="34"/>
     </row>
-    <row r="22" spans="2:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:30" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="12" t="str">
         <f>SEC_Processes!D20</f>
         <v>RHTDBLCHXE2</v>
@@ -5289,7 +5289,7 @@
       </c>
       <c r="AD22" s="34"/>
     </row>
-    <row r="23" spans="2:30" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:30" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B23" s="12" t="str">
         <f>SEC_Processes!D21</f>
         <v>RHTMBLCHXE2</v>
@@ -5368,7 +5368,7 @@
       </c>
       <c r="AD23" s="34"/>
     </row>
-    <row r="24" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B24" s="12" t="str">
         <f>SEC_Processes!D22</f>
         <v>RHTDBDHE1</v>
@@ -5424,11 +5424,11 @@
         <v>219</v>
       </c>
       <c r="X24" s="93">
-        <f t="shared" ref="X24:X33" si="3">V24/J21</f>
+        <f>V24/J21</f>
         <v>3.3058427586206895</v>
       </c>
       <c r="Y24" s="33" t="str">
-        <f t="shared" ref="Y24:Y30" si="4">D21</f>
+        <f t="shared" ref="Y24:Y26" si="3">D21</f>
         <v>RESWPE</v>
       </c>
       <c r="Z24" s="34"/>
@@ -5444,7 +5444,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B25" s="12" t="str">
         <f>SEC_Processes!D23</f>
         <v>RHTMBDHE1</v>
@@ -5500,11 +5500,11 @@
         <v>219</v>
       </c>
       <c r="X25" s="93">
+        <f>V25/J22</f>
+        <v>0.8138322580645162</v>
+      </c>
+      <c r="Y25" s="33" t="str">
         <f t="shared" si="3"/>
-        <v>0.8138322580645162</v>
-      </c>
-      <c r="Y25" s="33" t="str">
-        <f t="shared" si="4"/>
         <v>RESELCH</v>
       </c>
       <c r="Z25" s="34"/>
@@ -5520,7 +5520,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="26" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="str">
         <f>SEC_Processes!D24</f>
         <v>RCTDBAC</v>
@@ -5569,18 +5569,18 @@
         <v>218</v>
       </c>
       <c r="V26" s="93">
-        <f>O23*L23*N23</f>
+        <f t="shared" ref="V23:V30" si="4">O23*L23*N23</f>
         <v>2.6963280000000003</v>
       </c>
       <c r="W26" s="33" t="s">
         <v>219</v>
       </c>
       <c r="X26" s="93">
+        <f t="shared" ref="X24:X30" si="5">V26/J23</f>
+        <v>0.86978322580645173</v>
+      </c>
+      <c r="Y26" s="33" t="str">
         <f t="shared" si="3"/>
-        <v>0.86978322580645173</v>
-      </c>
-      <c r="Y26" s="33" t="str">
-        <f t="shared" si="4"/>
         <v>RESELCH</v>
       </c>
       <c r="Z26" s="34"/>
@@ -5588,7 +5588,7 @@
       <c r="AB26" s="93"/>
       <c r="AC26" s="94"/>
     </row>
-    <row r="27" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B27" s="12" t="str">
         <f>SEC_Processes!D25</f>
         <v>RCTMBAC</v>
@@ -5637,14 +5637,14 @@
         <v>218</v>
       </c>
       <c r="V27" s="93">
-        <f>O24*L24*N24</f>
+        <f t="shared" si="4"/>
         <v>3.31128</v>
       </c>
       <c r="W27" s="33" t="s">
         <v>219</v>
       </c>
       <c r="X27" s="93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.4492500000000001</v>
       </c>
       <c r="Y27" s="33" t="str">
@@ -5656,7 +5656,7 @@
       <c r="AB27" s="96"/>
       <c r="AC27" s="94"/>
     </row>
-    <row r="28" spans="2:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:30" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="12" t="str">
         <f>SEC_Processes!D26</f>
         <v>CHTLCHXE2</v>
@@ -5706,14 +5706,14 @@
         <v>218</v>
       </c>
       <c r="V28" s="93">
-        <f>O25*L25*N25</f>
+        <f t="shared" si="4"/>
         <v>2.7751679999999999</v>
       </c>
       <c r="W28" s="33" t="s">
         <v>219</v>
       </c>
       <c r="X28" s="93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.8318040816326531</v>
       </c>
       <c r="Y28" s="33" t="str">
@@ -5722,7 +5722,7 @@
       </c>
       <c r="Z28" s="95"/>
     </row>
-    <row r="29" spans="2:30" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:30" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B29" s="12" t="str">
         <f>SEC_Processes!D27</f>
         <v>CHTHCEBE1</v>
@@ -5779,7 +5779,7 @@
         <v>219</v>
       </c>
       <c r="X29" s="103">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.29755741935483865</v>
       </c>
       <c r="Y29" s="86" t="str">
@@ -5791,7 +5791,7 @@
       <c r="AB29" s="104"/>
       <c r="AC29" s="105"/>
     </row>
-    <row r="30" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="str">
         <f>SEC_Processes!D28</f>
         <v>CCTRBAC</v>
@@ -5848,7 +5848,7 @@
         <v>219</v>
       </c>
       <c r="X30" s="93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.25721549999999999</v>
       </c>
       <c r="Y30" s="33" t="str">
@@ -5860,7 +5860,7 @@
       <c r="AB30" s="95"/>
       <c r="AC30" s="97"/>
     </row>
-    <row r="31" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B31" s="30" t="str">
         <f>SEC_Processes!D29</f>
         <v>IPPT</v>
@@ -5907,7 +5907,7 @@
       <c r="AB31" s="95"/>
       <c r="AC31" s="97"/>
     </row>
-    <row r="32" spans="2:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:30" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="44" t="str">
         <f>SEC_Processes!D30</f>
         <v>FT-RESNGA</v>
@@ -5952,7 +5952,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="2:29" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:29" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B33" s="30" t="str">
         <f>SEC_Processes!D31</f>
         <v>FT-RESWPE</v>
@@ -6018,7 +6018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B34" s="12" t="str">
         <f>SEC_Processes!D32</f>
         <v>FT-RESELCH</v>
@@ -6058,18 +6058,18 @@
         <v>218</v>
       </c>
       <c r="V34" s="93">
-        <f t="shared" ref="V34:V35" si="5">O29*L29*N29</f>
+        <f>O29*L29*N29</f>
         <v>0.80732160000000008</v>
       </c>
       <c r="W34" s="33" t="s">
         <v>219</v>
       </c>
       <c r="X34" s="93">
-        <f t="shared" ref="X34:X35" si="6">V34/J29</f>
+        <f>V34/J29</f>
         <v>0.8237975510204083</v>
       </c>
       <c r="Y34" s="33" t="str">
-        <f t="shared" ref="Y34:Y35" si="7">D29</f>
+        <f t="shared" ref="Y34:Y35" si="6">D29</f>
         <v>COMDH</v>
       </c>
       <c r="Z34" s="34"/>
@@ -6085,7 +6085,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B35" s="12" t="str">
         <f>SEC_Processes!D33</f>
         <v>FT-RESELCA</v>
@@ -6125,7 +6125,7 @@
         <v>218</v>
       </c>
       <c r="V35" s="93">
-        <f t="shared" si="5"/>
+        <f>O30*L30*N30</f>
         <v>0.17029440000000001</v>
       </c>
       <c r="W35" s="33" t="s">
@@ -6136,7 +6136,7 @@
         <v>5.4933677419354843E-2</v>
       </c>
       <c r="Y35" s="33" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>COMELCH</v>
       </c>
       <c r="Z35" s="34"/>
@@ -6152,7 +6152,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="36" spans="2:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:29" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="12" t="str">
         <f>SEC_Processes!D34</f>
         <v>FT-RESHE</v>
@@ -6196,7 +6196,7 @@
       <c r="AB36" s="93"/>
       <c r="AC36" s="115"/>
     </row>
-    <row r="37" spans="2:29" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:29" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B37" s="12" t="str">
         <f>SEC_Processes!D35</f>
         <v>FT-COMELCH</v>
@@ -6240,7 +6240,7 @@
       <c r="AB37" s="103"/>
       <c r="AC37" s="103"/>
     </row>
-    <row r="38" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B38" s="12" t="str">
         <f>SEC_Processes!D36</f>
         <v>FT-COMHE</v>
@@ -6284,7 +6284,7 @@
       <c r="AB38" s="93"/>
       <c r="AC38" s="93"/>
     </row>
-    <row r="39" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B39" s="12" t="str">
         <f>SEC_Processes!D37</f>
         <v>FT-INDELC</v>
@@ -6328,7 +6328,7 @@
       <c r="AB39" s="95"/>
       <c r="AC39" s="95"/>
     </row>
-    <row r="40" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:29" x14ac:dyDescent="0.25">
       <c r="E40" s="31"/>
       <c r="F40" s="31"/>
       <c r="T40" s="116"/>
@@ -6342,7 +6342,7 @@
       <c r="AB40" s="95"/>
       <c r="AC40" s="95"/>
     </row>
-    <row r="41" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:29" x14ac:dyDescent="0.25">
       <c r="T41" s="116"/>
       <c r="U41" s="33"/>
       <c r="V41" s="93"/>
@@ -6354,7 +6354,7 @@
       <c r="AB41" s="95"/>
       <c r="AC41" s="95"/>
     </row>
-    <row r="42" spans="2:29" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:29" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B42" s="24" t="s">
         <v>124</v>
       </c>
@@ -6369,7 +6369,7 @@
       <c r="AB42" s="95"/>
       <c r="AC42" s="95"/>
     </row>
-    <row r="43" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:29" x14ac:dyDescent="0.25">
       <c r="T43" s="116"/>
       <c r="U43" s="33"/>
       <c r="V43" s="93"/>
@@ -6381,7 +6381,7 @@
       <c r="AB43" s="95"/>
       <c r="AC43" s="95"/>
     </row>
-    <row r="44" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:29" x14ac:dyDescent="0.25">
       <c r="T44" s="116"/>
       <c r="U44" s="95"/>
       <c r="V44" s="93"/>
@@ -6393,12 +6393,12 @@
       <c r="AB44" s="95"/>
       <c r="AC44" s="95"/>
     </row>
-    <row r="45" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B45" s="16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B46" s="15" t="s">
         <v>0</v>
       </c>
@@ -6413,7 +6413,7 @@
       </c>
       <c r="F46" s="43"/>
     </row>
-    <row r="47" spans="2:29" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:29" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="13" t="s">
         <v>46</v>
       </c>
@@ -6434,7 +6434,7 @@
       <c r="L47" s="56"/>
       <c r="M47" s="56"/>
     </row>
-    <row r="48" spans="2:29" ht="18" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:29" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B48" s="12" t="str">
         <f>SEC_Comm!D10</f>
         <v>RHD</v>
@@ -6461,7 +6461,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="49" spans="2:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="12" t="str">
         <f>SEC_Comm!D11</f>
         <v>RCD</v>
@@ -6486,7 +6486,7 @@
       <c r="L49" s="33"/>
       <c r="M49" s="56"/>
     </row>
-    <row r="50" spans="2:21" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:21" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B50" s="12" t="str">
         <f>SEC_Comm!D12</f>
         <v>RED</v>
@@ -6518,7 +6518,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="51" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B51" s="12" t="str">
         <f>SEC_Comm!D13</f>
         <v>RHM</v>
@@ -6551,7 +6551,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="52" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B52" s="12" t="str">
         <f>SEC_Comm!D14</f>
         <v>RCM</v>
@@ -6585,7 +6585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:21" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="12" t="str">
         <f>SEC_Comm!D15</f>
         <v>REM</v>
@@ -6619,7 +6619,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="54" spans="2:21" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:21" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B54" s="12" t="str">
         <f>SEC_Comm!D16</f>
         <v>CH</v>
@@ -6643,7 +6643,7 @@
       <c r="L54" s="33"/>
       <c r="M54" s="56"/>
     </row>
-    <row r="55" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B55" s="12" t="str">
         <f>SEC_Comm!D17</f>
         <v>CC</v>
@@ -6668,7 +6668,7 @@
       <c r="L55" s="33"/>
       <c r="M55" s="56"/>
     </row>
-    <row r="56" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B56" s="12" t="str">
         <f>SEC_Comm!D18</f>
         <v>IPP</v>
@@ -6692,7 +6692,7 @@
       <c r="L56" s="33"/>
       <c r="M56" s="56"/>
     </row>
-    <row r="57" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:21" x14ac:dyDescent="0.25">
       <c r="H57" s="56"/>
       <c r="I57" s="33"/>
       <c r="J57" s="33"/>
@@ -6700,7 +6700,7 @@
       <c r="L57" s="33"/>
       <c r="M57" s="56"/>
     </row>
-    <row r="58" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:21" x14ac:dyDescent="0.25">
       <c r="H58" s="56"/>
       <c r="I58" s="33"/>
       <c r="J58" s="33"/>
@@ -6708,7 +6708,7 @@
       <c r="L58" s="33"/>
       <c r="M58" s="56"/>
     </row>
-    <row r="59" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:21" x14ac:dyDescent="0.25">
       <c r="H59" s="56"/>
       <c r="I59" s="33"/>
       <c r="J59" s="33"/>
@@ -6716,7 +6716,7 @@
       <c r="L59" s="33"/>
       <c r="M59" s="56"/>
     </row>
-    <row r="60" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:21" x14ac:dyDescent="0.25">
       <c r="H60" s="56"/>
       <c r="I60" s="33"/>
       <c r="J60" s="33"/>
@@ -6724,7 +6724,7 @@
       <c r="L60" s="33"/>
       <c r="M60" s="56"/>
     </row>
-    <row r="61" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:21" x14ac:dyDescent="0.25">
       <c r="H61" s="56"/>
       <c r="I61" s="33"/>
       <c r="J61" s="33"/>
@@ -6732,7 +6732,7 @@
       <c r="L61" s="33"/>
       <c r="M61" s="56"/>
     </row>
-    <row r="62" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:21" x14ac:dyDescent="0.25">
       <c r="H62" s="56"/>
       <c r="I62" s="33"/>
       <c r="J62" s="33"/>
@@ -6740,7 +6740,7 @@
       <c r="L62" s="33"/>
       <c r="M62" s="56"/>
     </row>
-    <row r="63" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:21" x14ac:dyDescent="0.25">
       <c r="H63" s="56"/>
       <c r="I63" s="33"/>
       <c r="J63" s="33"/>
@@ -6748,7 +6748,7 @@
       <c r="L63" s="57"/>
       <c r="M63" s="56"/>
     </row>
-    <row r="64" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:21" x14ac:dyDescent="0.25">
       <c r="H64" s="56"/>
       <c r="I64" s="33"/>
       <c r="J64" s="33"/>
@@ -6756,7 +6756,7 @@
       <c r="L64" s="57"/>
       <c r="M64" s="56"/>
     </row>
-    <row r="65" spans="8:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H65" s="56"/>
       <c r="I65" s="33"/>
       <c r="J65" s="33"/>
@@ -6764,7 +6764,7 @@
       <c r="L65" s="57"/>
       <c r="M65" s="56"/>
     </row>
-    <row r="66" spans="8:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H66" s="56"/>
       <c r="I66" s="33"/>
       <c r="J66" s="33"/>
@@ -6772,7 +6772,7 @@
       <c r="L66" s="57"/>
       <c r="M66" s="56"/>
     </row>
-    <row r="67" spans="8:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H67" s="56"/>
       <c r="I67" s="33"/>
       <c r="J67" s="33"/>
@@ -6780,7 +6780,7 @@
       <c r="L67" s="57"/>
       <c r="M67" s="56"/>
     </row>
-    <row r="68" spans="8:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H68" s="56"/>
       <c r="I68" s="33"/>
       <c r="J68" s="33"/>
@@ -6788,7 +6788,7 @@
       <c r="L68" s="57"/>
       <c r="M68" s="56"/>
     </row>
-    <row r="69" spans="8:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H69" s="56"/>
       <c r="I69" s="56"/>
       <c r="J69" s="56"/>
@@ -6813,19 +6813,19 @@
       <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="45" t="s">
         <v>197</v>
       </c>
       <c r="C3" s="46"/>
       <c r="D3" s="46"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B4" s="47" t="s">
         <v>0</v>
       </c>
@@ -6834,7 +6834,7 @@
       </c>
       <c r="D4" s="53"/>
     </row>
-    <row r="5" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="49" t="s">
         <v>135</v>
       </c>
@@ -6843,7 +6843,7 @@
       </c>
       <c r="D5" s="54"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B6" s="51" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
RCI changed process with cooling commercial and residentcal heating multistorey to delate the dummies
</commit_message>
<xml_diff>
--- a/VT_SHR_RCI_V01.xlsx
+++ b/VT_SHR_RCI_V01.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jactat\Documents\Models\TIMES-Shire\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-Shire\Course_Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -798,7 +798,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="238">
   <si>
     <t>CommName</t>
   </si>
@@ -1491,6 +1491,27 @@
   </si>
   <si>
     <t>Energy Balance (PJ)</t>
+  </si>
+  <si>
+    <t>j12 was 21</t>
+  </si>
+  <si>
+    <t>j18 was 25</t>
+  </si>
+  <si>
+    <t>027 was 145</t>
+  </si>
+  <si>
+    <t>030 was 18</t>
+  </si>
+  <si>
+    <t>n30 was 0.3</t>
+  </si>
+  <si>
+    <t>j15 was 21</t>
+  </si>
+  <si>
+    <t>e54 was 4, now 3.9</t>
   </si>
 </sst>
 </file>
@@ -1620,7 +1641,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1690,6 +1711,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1925,7 +1952,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2114,6 +2141,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4292,8 +4321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AD69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" topLeftCell="I7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4337,6 +4366,23 @@
       <c r="B3" s="11" t="s">
         <v>35</v>
       </c>
+      <c r="J3" t="s">
+        <v>233</v>
+      </c>
+      <c r="L3" t="s">
+        <v>234</v>
+      </c>
+      <c r="M3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>231</v>
+      </c>
+      <c r="L4" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="5" spans="2:30" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
@@ -4345,6 +4391,12 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
+      <c r="J5" t="s">
+        <v>232</v>
+      </c>
+      <c r="L5" t="s">
+        <v>236</v>
+      </c>
       <c r="R5" s="34"/>
       <c r="S5" s="35"/>
       <c r="T5" s="36"/>
@@ -4653,8 +4705,8 @@
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
-      <c r="J12" s="100">
-        <v>21</v>
+      <c r="J12" s="118">
+        <v>22</v>
       </c>
       <c r="K12" s="12">
         <v>100</v>
@@ -4678,7 +4730,7 @@
       </c>
       <c r="U12" s="101">
         <f>J12*SUM(V29)</f>
-        <v>19.370987999999997</v>
+        <v>20.293415999999997</v>
       </c>
       <c r="V12" s="33">
         <f t="shared" ref="V12:V18" si="1">E49</f>
@@ -4842,8 +4894,8 @@
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
-      <c r="J15" s="74">
-        <v>21</v>
+      <c r="J15" s="118">
+        <v>22</v>
       </c>
       <c r="K15" s="12">
         <v>100</v>
@@ -4867,9 +4919,9 @@
       </c>
       <c r="U15" s="57">
         <f>J15*SUM(V30)</f>
-        <v>17.284881599999999</v>
-      </c>
-      <c r="V15" s="33">
+        <v>21.2300352</v>
+      </c>
+      <c r="V15" s="119">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
@@ -5031,7 +5083,7 @@
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
-      <c r="J18" s="100">
+      <c r="J18" s="118">
         <v>25</v>
       </c>
       <c r="K18" s="12">
@@ -5056,7 +5108,7 @@
       </c>
       <c r="U18" s="57">
         <f>J18*SUM(V35)</f>
-        <v>4.2573600000000003</v>
+        <v>23.651999999999997</v>
       </c>
       <c r="V18" s="33">
         <f t="shared" si="1"/>
@@ -5437,7 +5489,7 @@
       </c>
       <c r="AB24" s="93">
         <f>SUM(X25:X26,X29:X30)+V13/J13+V16/J16</f>
-        <v>6.0249900003864099</v>
+        <v>6.0693375003864105</v>
       </c>
       <c r="AC24" s="94">
         <f>T51</f>
@@ -5569,14 +5621,14 @@
         <v>218</v>
       </c>
       <c r="V26" s="93">
-        <f t="shared" ref="V23:V30" si="4">O23*L23*N23</f>
+        <f t="shared" ref="V26:V28" si="4">O23*L23*N23</f>
         <v>2.6963280000000003</v>
       </c>
       <c r="W26" s="33" t="s">
         <v>219</v>
       </c>
       <c r="X26" s="93">
-        <f t="shared" ref="X24:X30" si="5">V26/J23</f>
+        <f t="shared" ref="X26:X30" si="5">V26/J23</f>
         <v>0.86978322580645173</v>
       </c>
       <c r="Y26" s="33" t="str">
@@ -5623,8 +5675,8 @@
       <c r="N27" s="100">
         <v>0.18</v>
       </c>
-      <c r="O27" s="100">
-        <v>145</v>
+      <c r="O27" s="118">
+        <v>170</v>
       </c>
       <c r="P27" s="12"/>
       <c r="S27" s="34" t="s">
@@ -5824,11 +5876,11 @@
         <v>3.1536000000000002E-2</v>
       </c>
       <c r="M30" s="30"/>
-      <c r="N30" s="74">
+      <c r="N30" s="118">
         <v>0.3</v>
       </c>
-      <c r="O30" s="74">
-        <v>18</v>
+      <c r="O30" s="118">
+        <v>100</v>
       </c>
       <c r="P30" s="30"/>
       <c r="S30" s="34" t="s">
@@ -5842,14 +5894,14 @@
       </c>
       <c r="V30" s="93">
         <f>O27*L27*N27</f>
-        <v>0.82308959999999998</v>
+        <v>0.96500160000000001</v>
       </c>
       <c r="W30" s="33" t="s">
         <v>219</v>
       </c>
       <c r="X30" s="93">
         <f t="shared" si="5"/>
-        <v>0.25721549999999999</v>
+        <v>0.30156299999999997</v>
       </c>
       <c r="Y30" s="33" t="str">
         <f>D27</f>
@@ -6078,7 +6130,7 @@
       </c>
       <c r="AB34" s="93">
         <f>SUM(X33,X35)</f>
-        <v>0.47609187096774203</v>
+        <v>0.72634529032258066</v>
       </c>
       <c r="AC34" s="94">
         <f>U51</f>
@@ -6126,14 +6178,14 @@
       </c>
       <c r="V35" s="93">
         <f>O30*L30*N30</f>
-        <v>0.17029440000000001</v>
+        <v>0.94607999999999992</v>
       </c>
       <c r="W35" s="33" t="s">
         <v>219</v>
       </c>
       <c r="X35" s="93">
         <f>V35/J30</f>
-        <v>5.4933677419354843E-2</v>
+        <v>0.30518709677419353</v>
       </c>
       <c r="Y35" s="33" t="str">
         <f t="shared" si="6"/>

</xml_diff>